<commit_message>
BUGFIX: GDD methods now working and verified
</commit_message>
<xml_diff>
--- a/test/test_data/tables/Irrigation_lookup_CDL.xlsx
+++ b/test/test_data/tables/Irrigation_lookup_CDL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/OWC_Aura_SSD_1TB/Users/SMWData/git_repos/swb2_examples/central_sands/std_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\swb_development\git\swb2\test\test_data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1251B07E-9F95-4596-9294-6ADD833C0925}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="9444" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Irrigation_table_05_07_2015b_SW" sheetId="1" r:id="rId1"/>
@@ -506,7 +507,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
@@ -567,6 +568,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -834,26 +838,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="27.34765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.84765625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.84765625" style="3"/>
     <col min="10" max="10" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="3"/>
-    <col min="16" max="16" width="10.83203125" style="2"/>
-    <col min="36" max="37" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="10.84765625" style="3"/>
+    <col min="16" max="16" width="10.84765625" style="2"/>
+    <col min="36" max="37" width="10.84765625" style="1"/>
     <col min="41" max="41" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -921,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1165,7 +1169,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -1290,7 +1294,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1391,7 +1395,7 @@
         <v>50</v>
       </c>
       <c r="AH5">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI5">
         <v>0.5</v>
@@ -1415,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1516,7 +1520,7 @@
         <v>50</v>
       </c>
       <c r="AH6">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI6">
         <v>0.5</v>
@@ -1540,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1641,7 +1645,7 @@
         <v>50</v>
       </c>
       <c r="AH7">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI7">
         <v>0.5</v>
@@ -1665,7 +1669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>50</v>
       </c>
       <c r="AH8">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI8">
         <v>0.45</v>
@@ -1790,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A9">
         <v>12</v>
       </c>
@@ -1891,7 +1895,7 @@
         <v>50</v>
       </c>
       <c r="AH9">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI9">
         <v>0.5</v>
@@ -1915,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A10">
         <v>21</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>50</v>
       </c>
       <c r="AH10">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI10">
         <v>0.55000000000000004</v>
@@ -2040,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A11">
         <v>23</v>
       </c>
@@ -2141,7 +2145,7 @@
         <v>50</v>
       </c>
       <c r="AH11">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI11">
         <v>0.55000000000000004</v>
@@ -2165,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A12">
         <v>24</v>
       </c>
@@ -2266,7 +2270,7 @@
         <v>50</v>
       </c>
       <c r="AH12">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI12">
         <v>0.55000000000000004</v>
@@ -2290,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A13">
         <v>26</v>
       </c>
@@ -2391,7 +2395,7 @@
         <v>50</v>
       </c>
       <c r="AH13">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI13">
         <v>0.55000000000000004</v>
@@ -2415,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A14">
         <v>27</v>
       </c>
@@ -2516,7 +2520,7 @@
         <v>50</v>
       </c>
       <c r="AH14">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI14">
         <v>0.55000000000000004</v>
@@ -2540,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A15">
         <v>28</v>
       </c>
@@ -2641,7 +2645,7 @@
         <v>50</v>
       </c>
       <c r="AH15">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI15">
         <v>0.55000000000000004</v>
@@ -2665,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A16">
         <v>29</v>
       </c>
@@ -2766,7 +2770,7 @@
         <v>50</v>
       </c>
       <c r="AH16">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI16">
         <v>0.55000000000000004</v>
@@ -2790,7 +2794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A17">
         <v>30</v>
       </c>
@@ -2891,7 +2895,7 @@
         <v>50</v>
       </c>
       <c r="AH17">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI17">
         <v>0.55000000000000004</v>
@@ -2915,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A18">
         <v>32</v>
       </c>
@@ -3016,7 +3020,7 @@
         <v>50</v>
       </c>
       <c r="AH18">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI18">
         <v>0.55000000000000004</v>
@@ -3040,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A19">
         <v>36</v>
       </c>
@@ -3141,7 +3145,7 @@
         <v>50</v>
       </c>
       <c r="AH19">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI19">
         <v>0.6</v>
@@ -3165,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A20">
         <v>37</v>
       </c>
@@ -3266,7 +3270,7 @@
         <v>50</v>
       </c>
       <c r="AH20">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI20">
         <v>0.55000000000000004</v>
@@ -3290,7 +3294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A21">
         <v>38</v>
       </c>
@@ -3391,7 +3395,7 @@
         <v>50</v>
       </c>
       <c r="AH21">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI21">
         <v>0.55000000000000004</v>
@@ -3415,7 +3419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A22">
         <v>41</v>
       </c>
@@ -3516,7 +3520,7 @@
         <v>50</v>
       </c>
       <c r="AH22">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI22">
         <v>0.55000000000000004</v>
@@ -3540,7 +3544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A23">
         <v>42</v>
       </c>
@@ -3641,7 +3645,7 @@
         <v>50</v>
       </c>
       <c r="AH23">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI23">
         <v>0.55000000000000004</v>
@@ -3665,7 +3669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A24">
         <v>43</v>
       </c>
@@ -3766,7 +3770,7 @@
         <v>50</v>
       </c>
       <c r="AH24">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI24">
         <v>0.55000000000000004</v>
@@ -3790,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A25">
         <v>47</v>
       </c>
@@ -3891,7 +3895,7 @@
         <v>50</v>
       </c>
       <c r="AH25">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI25">
         <v>0.55000000000000004</v>
@@ -3915,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A26">
         <v>49</v>
       </c>
@@ -4016,7 +4020,7 @@
         <v>50</v>
       </c>
       <c r="AH26">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI26">
         <v>0.55000000000000004</v>
@@ -4040,7 +4044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A27">
         <v>50</v>
       </c>
@@ -4141,7 +4145,7 @@
         <v>50</v>
       </c>
       <c r="AH27">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI27">
         <v>0.35</v>
@@ -4165,7 +4169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A28">
         <v>53</v>
       </c>
@@ -4266,7 +4270,7 @@
         <v>50</v>
       </c>
       <c r="AH28">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI28">
         <v>0.35</v>
@@ -4290,7 +4294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A29">
         <v>57</v>
       </c>
@@ -4391,7 +4395,7 @@
         <v>50</v>
       </c>
       <c r="AH29">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI29">
         <v>0.4</v>
@@ -4415,7 +4419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A30">
         <v>58</v>
       </c>
@@ -4516,7 +4520,7 @@
         <v>50</v>
       </c>
       <c r="AH30">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI30">
         <v>0.55000000000000004</v>
@@ -4540,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A31">
         <v>59</v>
       </c>
@@ -4641,7 +4645,7 @@
         <v>50</v>
       </c>
       <c r="AH31">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI31">
         <v>1</v>
@@ -4665,7 +4669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A32">
         <v>61</v>
       </c>
@@ -4766,7 +4770,7 @@
         <v>50</v>
       </c>
       <c r="AH32">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI32">
         <v>1</v>
@@ -4790,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A33">
         <v>70</v>
       </c>
@@ -4891,7 +4895,7 @@
         <v>50</v>
       </c>
       <c r="AH33">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI33">
         <v>1</v>
@@ -4915,7 +4919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A34">
         <v>92</v>
       </c>
@@ -5016,7 +5020,7 @@
         <v>50</v>
       </c>
       <c r="AH34">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI34">
         <v>1</v>
@@ -5040,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:41" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:41" s="4" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A35" s="4">
         <v>111</v>
       </c>
@@ -5140,8 +5144,8 @@
       <c r="AG35" s="4">
         <v>50</v>
       </c>
-      <c r="AH35" s="4">
-        <v>130</v>
+      <c r="AH35">
+        <v>86</v>
       </c>
       <c r="AI35" s="4">
         <v>1</v>
@@ -5165,7 +5169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A36">
         <v>121</v>
       </c>
@@ -5266,7 +5270,7 @@
         <v>50</v>
       </c>
       <c r="AH36">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI36">
         <v>1</v>
@@ -5290,7 +5294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A37">
         <v>122</v>
       </c>
@@ -5391,7 +5395,7 @@
         <v>50</v>
       </c>
       <c r="AH37">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI37">
         <v>1</v>
@@ -5415,7 +5419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A38">
         <v>123</v>
       </c>
@@ -5516,7 +5520,7 @@
         <v>50</v>
       </c>
       <c r="AH38">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI38">
         <v>1</v>
@@ -5540,7 +5544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A39">
         <v>124</v>
       </c>
@@ -5641,7 +5645,7 @@
         <v>50</v>
       </c>
       <c r="AH39">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI39">
         <v>1</v>
@@ -5665,7 +5669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A40">
         <v>131</v>
       </c>
@@ -5766,7 +5770,7 @@
         <v>50</v>
       </c>
       <c r="AH40">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI40">
         <v>1</v>
@@ -5790,7 +5794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A41">
         <v>141</v>
       </c>
@@ -5891,7 +5895,7 @@
         <v>50</v>
       </c>
       <c r="AH41">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI41">
         <v>1</v>
@@ -5915,7 +5919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A42">
         <v>142</v>
       </c>
@@ -6016,7 +6020,7 @@
         <v>50</v>
       </c>
       <c r="AH42">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI42">
         <v>1</v>
@@ -6040,7 +6044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A43">
         <v>143</v>
       </c>
@@ -6141,7 +6145,7 @@
         <v>50</v>
       </c>
       <c r="AH43">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI43">
         <v>1</v>
@@ -6165,7 +6169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A44">
         <v>151</v>
       </c>
@@ -6266,7 +6270,7 @@
         <v>50</v>
       </c>
       <c r="AH44">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI44">
         <v>1</v>
@@ -6290,7 +6294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A45">
         <v>152</v>
       </c>
@@ -6391,7 +6395,7 @@
         <v>50</v>
       </c>
       <c r="AH45">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI45">
         <v>1</v>
@@ -6415,7 +6419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A46">
         <v>171</v>
       </c>
@@ -6516,7 +6520,7 @@
         <v>50</v>
       </c>
       <c r="AH46">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI46">
         <v>1</v>
@@ -6540,7 +6544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A47">
         <v>176</v>
       </c>
@@ -6641,7 +6645,7 @@
         <v>50</v>
       </c>
       <c r="AH47">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI47">
         <v>1</v>
@@ -6665,7 +6669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A48">
         <v>181</v>
       </c>
@@ -6766,7 +6770,7 @@
         <v>50</v>
       </c>
       <c r="AH48">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI48">
         <v>1</v>
@@ -6790,7 +6794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A49">
         <v>182</v>
       </c>
@@ -6891,7 +6895,7 @@
         <v>50</v>
       </c>
       <c r="AH49">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI49">
         <v>0.55000000000000004</v>
@@ -6915,7 +6919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A50">
         <v>190</v>
       </c>
@@ -7016,7 +7020,7 @@
         <v>50</v>
       </c>
       <c r="AH50">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI50">
         <v>1</v>
@@ -7040,7 +7044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A51">
         <v>195</v>
       </c>
@@ -7141,7 +7145,7 @@
         <v>50</v>
       </c>
       <c r="AH51">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI51">
         <v>1</v>
@@ -7165,7 +7169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A52">
         <v>205</v>
       </c>
@@ -7266,7 +7270,7 @@
         <v>50</v>
       </c>
       <c r="AH52">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI52">
         <v>0.35</v>
@@ -7290,7 +7294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A53">
         <v>206</v>
       </c>
@@ -7391,7 +7395,7 @@
         <v>50</v>
       </c>
       <c r="AH53">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI53">
         <v>0.35</v>
@@ -7415,7 +7419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A54">
         <v>207</v>
       </c>
@@ -7516,7 +7520,7 @@
         <v>50</v>
       </c>
       <c r="AH54">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI54">
         <v>0.45</v>
@@ -7540,7 +7544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A55">
         <v>221</v>
       </c>
@@ -7641,7 +7645,7 @@
         <v>50</v>
       </c>
       <c r="AH55">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI55">
         <v>0.45</v>
@@ -7665,7 +7669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A56">
         <v>225</v>
       </c>
@@ -7766,7 +7770,7 @@
         <v>50</v>
       </c>
       <c r="AH56">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI56">
         <v>0.55000000000000004</v>
@@ -7790,7 +7794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A57">
         <v>226</v>
       </c>
@@ -7891,7 +7895,7 @@
         <v>50</v>
       </c>
       <c r="AH57">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI57">
         <v>0.55000000000000004</v>
@@ -7915,7 +7919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A58">
         <v>241</v>
       </c>
@@ -8016,7 +8020,7 @@
         <v>50</v>
       </c>
       <c r="AH58">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI58">
         <v>0.55000000000000004</v>
@@ -8040,7 +8044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A59">
         <v>242</v>
       </c>
@@ -8141,7 +8145,7 @@
         <v>50</v>
       </c>
       <c r="AH59">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI59">
         <v>0.45</v>
@@ -8165,7 +8169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A60">
         <v>243</v>
       </c>
@@ -8266,7 +8270,7 @@
         <v>50</v>
       </c>
       <c r="AH60">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI60">
         <v>0.45</v>
@@ -8290,7 +8294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A61">
         <v>250</v>
       </c>
@@ -8391,7 +8395,7 @@
         <v>50</v>
       </c>
       <c r="AH61">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI61">
         <v>0.5</v>
@@ -8415,7 +8419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A62">
         <v>251</v>
       </c>
@@ -8516,7 +8520,7 @@
         <v>50</v>
       </c>
       <c r="AH62">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI62">
         <v>0.1</v>
@@ -8540,7 +8544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.6">
       <c r="A63">
         <v>252</v>
       </c>
@@ -8641,7 +8645,7 @@
         <v>50</v>
       </c>
       <c r="AH63">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="AI63">
         <v>0.1</v>

</xml_diff>